<commit_message>
testing ctd model filtered
</commit_message>
<xml_diff>
--- a/out/Q2A Excel Sheet.xlsx
+++ b/out/Q2A Excel Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrysun_1/Desktop/Duke/2024-2025/Summer 2024/fishics/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FA7C5-D8BC-D542-8982-10C44F80D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DE1A5B-5B05-784D-B8A1-3904704D6601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4DACB700-5750-884D-ACB6-995FA53AAEA5}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +94,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFDFDFD"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1717,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE4A346-A9EB-544B-B244-C983DCFFA6D3}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1879,6 +1886,9 @@
         <v>0.102202</v>
       </c>
     </row>
+    <row r="22" spans="4:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>